<commit_message>
Original import tree update
</commit_message>
<xml_diff>
--- a/Database_edition/source_import/Example_bw/Livebox_6.xlsx
+++ b/Database_edition/source_import/Example_bw/Livebox_6.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dokuwiki\data\Wiki-on-processes-and-products-for-LCA\Database_edition\source_import\Example_bw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects_git\FY25\LCA\Wiki-on-processes-and-products-for-LCA\Database_edition\source_import\Example_bw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FEFA99-7CE9-4052-B39E-1DD5BD716D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C27B8C-A0F4-4B82-8134-3060E9D7E596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary_LCI" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="90">
   <si>
     <t>Database</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>printed circuit board production</t>
+  </si>
+  <si>
+    <t>XX</t>
   </si>
 </sst>
 </file>
@@ -944,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB43B447-921B-4B79-B848-5DFD49186505}">
   <dimension ref="A1:K175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3048,7 +3051,9 @@
       <c r="A122" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="B122" s="33"/>
+      <c r="B122" s="33" t="s">
+        <v>89</v>
+      </c>
       <c r="C122" s="25" t="s">
         <v>87</v>
       </c>
@@ -3060,8 +3065,12 @@
         <v>86</v>
       </c>
       <c r="F122" s="25"/>
-      <c r="G122" s="25"/>
-      <c r="H122" s="25"/>
+      <c r="G122" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H122" s="24" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="123" spans="1:11" s="22" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A123" s="11" t="str">
@@ -3189,14 +3198,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bda8bc8f-1fd2-4e78-a6bc-9ebf19518310">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="befa33bd-d94f-430f-aef1-5ab98afa7ccf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3389,21 +3396,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bda8bc8f-1fd2-4e78-a6bc-9ebf19518310">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="befa33bd-d94f-430f-aef1-5ab98afa7ccf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC11A217-A777-4951-9D25-5870F10F0905}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EB2EA89-4A79-404A-B8EF-E6B59010D46B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bda8bc8f-1fd2-4e78-a6bc-9ebf19518310"/>
-    <ds:schemaRef ds:uri="befa33bd-d94f-430f-aef1-5ab98afa7ccf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3428,9 +3434,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EB2EA89-4A79-404A-B8EF-E6B59010D46B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC11A217-A777-4951-9D25-5870F10F0905}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bda8bc8f-1fd2-4e78-a6bc-9ebf19518310"/>
+    <ds:schemaRef ds:uri="befa33bd-d94f-430f-aef1-5ab98afa7ccf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>